<commit_message>
update test case and report level 1
</commit_message>
<xml_diff>
--- a/config/testcases/Report_MC.RS01DienThe(Clone).xlsx
+++ b/config/testcases/Report_MC.RS01DienThe(Clone).xlsx
@@ -283,18 +283,6 @@
     <t>ItemsDrag/$.path,SyncItem_Image(Clone)</t>
   </si>
   <si>
-    <t>Kiểm tra text hoàn chỉnh</t>
-  </si>
-  <si>
-    <t>Mic-Normal</t>
-  </si>
-  <si>
-    <t>GamePlaySpeak//Text</t>
-  </si>
-  <si>
-    <t>$.act[?(@.game_name=="MC.RS01DienThe(Clone)")].turn[0].word[?(@.type=='question')].text</t>
-  </si>
-  <si>
     <t>TS5</t>
   </si>
   <si>
@@ -308,6 +296,18 @@
   </si>
   <si>
     <t>$.act[?(@.game_name=="MC.RS01DienThe(Clone)")].turn[1].word[?(@.type=='question')].audio[*].file_path</t>
+  </si>
+  <si>
+    <t>Kiểm tra text hoàn chỉnh</t>
+  </si>
+  <si>
+    <t>Mic-Normal</t>
+  </si>
+  <si>
+    <t>GamePlaySpeak//Text</t>
+  </si>
+  <si>
+    <t>$.act[?(@.game_name=="MC.RS01DienThe(Clone)")].turn[0].word[?(@.type=='question')].text</t>
   </si>
   <si>
     <t>TS6</t>
@@ -1958,30 +1958,28 @@
         <v>23</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="28" t="s">
         <v>88</v>
       </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="16"/>
       <c r="G15" s="24" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="16"/>
+        <v>90</v>
+      </c>
+      <c r="J15" s="26" t="s">
+        <v>91</v>
+      </c>
       <c r="K15" s="26" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -1992,28 +1990,30 @@
         <v>23</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C16" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="D16" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="F16" s="16"/>
       <c r="G16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="16"/>
+      <c r="K16" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="K16" s="26" t="s">
-        <v>53</v>
       </c>
       <c r="L16" s="16"/>
       <c r="M16" s="16"/>
@@ -2102,10 +2102,10 @@
         <v>52</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L19" s="16"/>
       <c r="M19" s="16"/>
@@ -2511,67 +2511,67 @@
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
     </row>
-    <row r="33" ht="36.75" customHeight="1">
+    <row r="33" ht="48.0" customHeight="1">
       <c r="A33" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="28" t="s">
         <v>88</v>
       </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28"/>
       <c r="F33" s="16"/>
       <c r="G33" s="24" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J33" s="26"/>
+        <v>90</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>91</v>
+      </c>
       <c r="K33" s="26" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
     </row>
-    <row r="34" ht="48.0" customHeight="1">
+    <row r="34" ht="36.75" customHeight="1">
       <c r="A34" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="28"/>
+      <c r="D34" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>93</v>
+      </c>
       <c r="F34" s="16"/>
       <c r="G34" s="24" t="s">
         <v>12</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="J34" s="26" t="s">
-        <v>95</v>
-      </c>
+      <c r="J34" s="26"/>
       <c r="K34" s="26" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
@@ -2582,7 +2582,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C35" s="43" t="s">
         <v>97</v>
@@ -2681,8 +2681,8 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20 H32">
       <formula1>Keywords!$A$2:$A182</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H15:H16">
-      <formula1>Keywords!$A$2:$A180</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33">
+      <formula1>Keywords!$A$2:$A198</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H27:H29">
       <formula1>Keywords!$A$2:$A195</formula1>
@@ -2702,19 +2702,19 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H3:H5 H19">
       <formula1>Keywords!$A$2:$A176</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H17:H18 H33:H34">
-      <formula1>Keywords!$A$2:$A181</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H16:H18">
+      <formula1>Keywords!$A$2:$A180</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G37">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H30:H31">
-      <formula1>Keywords!$A$2:$A196</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H15 H30:H31">
+      <formula1>Keywords!$A$2:$A181</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H37">
       <formula1>Keywords!$A$2:$A187</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2 H14 H35:H36">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2 H14 H34:H36">
       <formula1>Keywords!$A$2:$A165</formula1>
     </dataValidation>
   </dataValidations>
@@ -6615,8 +6615,8 @@
         <v>deFindAnswerDienThe</v>
       </c>
       <c r="B101" s="52" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"locator(ảnh),component,property[,strReplace,strAdd],locator1(text),expect")</f>
-        <v>locator(ảnh),component,property[,strReplace,strAdd],locator1(text),expect</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"element(ảnh),component,property[,strReplace,strAdd],element1(text),expect")</f>
+        <v>element(ảnh),component,property[,strReplace,strAdd],element1(text),expect</v>
       </c>
       <c r="C101" s="52" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"void")</f>
@@ -6729,8 +6729,8 @@
         <v>swipeMap</v>
       </c>
       <c r="B104" s="52" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"locator,component,property,key,expect")</f>
-        <v>locator,component,property,key,expect</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"element,component,property,key,expect")</f>
+        <v>element,component,property,key,expect</v>
       </c>
       <c r="C104" s="52" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"void")</f>
@@ -6764,12 +6764,24 @@
       <c r="Z104" s="52"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="52"/>
-      <c r="B105" s="52"/>
-      <c r="C105" s="52"/>
+      <c r="A105" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"comPairImage")</f>
+        <v>comPairImage</v>
+      </c>
+      <c r="B105" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"element,expect")</f>
+        <v>element,expect</v>
+      </c>
+      <c r="C105" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"String")</f>
+        <v>String</v>
+      </c>
       <c r="D105" s="52"/>
       <c r="E105" s="52"/>
-      <c r="F105" s="52"/>
+      <c r="F105" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"trả về true or false dùng trong những TH check ảnh có hoặc k tùy data")</f>
+        <v>trả về true or false dùng trong những TH check ảnh có hoặc k tùy data</v>
+      </c>
       <c r="G105" s="52"/>
       <c r="H105" s="52"/>
       <c r="I105" s="52"/>
@@ -6792,12 +6804,24 @@
       <c r="Z105" s="52"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="52"/>
-      <c r="B106" s="52"/>
-      <c r="C106" s="52"/>
+      <c r="A106" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"skipLesson")</f>
+        <v>skipLesson</v>
+      </c>
+      <c r="B106" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"element")</f>
+        <v>element</v>
+      </c>
+      <c r="C106" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"void")</f>
+        <v>void</v>
+      </c>
       <c r="D106" s="52"/>
       <c r="E106" s="52"/>
-      <c r="F106" s="52"/>
+      <c r="F106" s="52" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"sử dụng với những nút có thể onclick()")</f>
+        <v>sử dụng với những nút có thể onclick()</v>
+      </c>
       <c r="G106" s="52"/>
       <c r="H106" s="52"/>
       <c r="I106" s="52"/>

</xml_diff>